<commit_message>
add graus de liberdade
</commit_message>
<xml_diff>
--- a/entradas.xlsx
+++ b/entradas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Insper\5-Semestre\TransCal\P2\TransCal-P2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A0A904-C04A-4FC0-80E5-595C9A354F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEBDA2B-B7E7-4705-9AD4-7624F256519A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,8 +46,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -77,7 +85,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -388,21 +396,65 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
não estou seguro quanto ao grau de liberdade, mas acho que os calculos de L , s e c estão certos
</commit_message>
<xml_diff>
--- a/entradas.xlsx
+++ b/entradas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Insper\5-Semestre\TransCal\P2\TransCal-P2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEBDA2B-B7E7-4705-9AD4-7624F256519A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D897A4-F39E-4C83-8B51-3723AA454457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -369,7 +369,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -400,9 +400,15 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
     </row>
@@ -411,10 +417,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>0.4</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -422,33 +434,20 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>0.3</v>
       </c>
       <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
+        <v>0.4</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D11" s="1"/>

</xml_diff>

<commit_message>
adicionando matriz  de rigidez
</commit_message>
<xml_diff>
--- a/entradas.xlsx
+++ b/entradas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Insper\5-Semestre\TransCal\P2\TransCal-P2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791A099F-7236-4702-B736-226E785AA465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC956723-9F3C-408B-BD1C-29FA78CD2494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +61,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,9 +95,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,13 +393,14 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -396,55 +421,58 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
+      <c r="D2" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="E2" s="5">
+        <v>2.0000000000000001E-4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>0.4</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
+      <c r="D3" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2.0000000000000001E-4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>0.3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>0.4</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
+      <c r="D4" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="E4" s="5">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D5" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D10" s="1"/>
@@ -453,6 +481,7 @@
       <c r="D11" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
ajuste do gráfico e adicionando função de acrescentar estruturas de apoio
</commit_message>
<xml_diff>
--- a/entradas.xlsx
+++ b/entradas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Insper\5-Semestre\TransCal\P2\TransCal-P2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC956723-9F3C-408B-BD1C-29FA78CD2494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77E23DD-05B7-475C-9639-2EC357FB9348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Nós</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Área</t>
+  </si>
+  <si>
+    <t>Tipo de Apoio</t>
   </si>
 </sst>
 </file>
@@ -390,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -403,7 +406,7 @@
     <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,8 +422,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -436,8 +442,11 @@
       <c r="E2" s="5">
         <v>2.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -453,8 +462,11 @@
       <c r="E3" s="5">
         <v>2.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -470,14 +482,17 @@
       <c r="E4" s="5">
         <v>2.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D5" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D11" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adicionando matriz de rigidez global
</commit_message>
<xml_diff>
--- a/entradas.xlsx
+++ b/entradas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Insper\5-Semestre\TransCal\P2\TransCal-P2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77E23DD-05B7-475C-9639-2EC357FB9348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34EA16C6-A84B-4768-9114-11A93C7C6F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F5" sqref="A5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -487,7 +487,12 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="2"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D10" s="1"/>

</xml_diff>

<commit_message>
agora vai no Julião
</commit_message>
<xml_diff>
--- a/entradas.xlsx
+++ b/entradas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Insper\5-Semestre\TransCal\P2\TransCal-P2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5576EAC7-79B3-4B12-A305-70145EF50783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEBFF2E-3C0F-4B92-A191-832DECAE17EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -435,7 +435,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -474,7 +474,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -531,7 +531,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -678,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
@@ -706,7 +706,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -720,7 +720,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>